<commit_message>
Small changes to results
</commit_message>
<xml_diff>
--- a/fs_mol/outputs/test/aggregate_across_targets.xlsx
+++ b/fs_mol/outputs/test/aggregate_across_targets.xlsx
@@ -1,28 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phevo\Documents\Harvard\Junior-Year\CS288\ersilia-fsmol\fs_mol\outputs\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F75F96-2B75-401E-B1D6-9EB750AD9542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>4_train (PN)</t>
   </si>
   <si>
+    <t>4_train (GNN-MT)</t>
+  </si>
+  <si>
     <t>4_train (RF)</t>
   </si>
   <si>
     <t>4_train (PN) std</t>
+  </si>
+  <si>
+    <t>4_train (GNN-MT) std</t>
   </si>
   <si>
     <t>4_train (RF) std</t>
@@ -82,8 +94,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,13 +158,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +210,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -224,6 +244,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -258,9 +279,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,16 +455,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.62890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.62890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.20703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.62890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.62890625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -492,217 +529,247 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <v>0.2221029411764706</v>
+        <v>0.22210294117647059</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>0.1127058823529411</v>
       </c>
-      <c r="D2">
-        <v>0.0147381623389696</v>
-      </c>
       <c r="E2">
-        <v>0.0140127786282842</v>
+        <v>1.47381623389696E-2</v>
       </c>
       <c r="F2">
-        <v>0.2075645161290322</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.1795888888888889</v>
+        <v>1.4012778628284201E-2</v>
       </c>
       <c r="H2">
-        <v>0.1795888888888889</v>
+        <v>0.2077258064516129</v>
       </c>
       <c r="I2">
-        <v>0.0149087308799856</v>
+        <v>0.17977407407407409</v>
       </c>
       <c r="J2">
-        <v>0.0135702417521743</v>
+        <v>0.156074193548387</v>
       </c>
       <c r="K2">
-        <v>0.0135702417521743</v>
+        <v>1.4898701032745799E-2</v>
       </c>
       <c r="L2">
-        <v>0.192171568627451</v>
+        <v>1.35619692803948E-2</v>
       </c>
       <c r="M2">
+        <v>1.3370374111326E-2</v>
+      </c>
+      <c r="N2">
+        <v>0.19217156862745099</v>
+      </c>
+      <c r="O2">
         <v>0.1661186274509803</v>
       </c>
-      <c r="N2">
-        <v>0.1661186274509803</v>
-      </c>
-      <c r="O2">
-        <v>0.0118697072972182</v>
-      </c>
       <c r="P2">
-        <v>0.0107955207220888</v>
+        <v>0.18568921568627439</v>
       </c>
       <c r="Q2">
-        <v>0.0107955207220888</v>
+        <v>1.18697072972182E-2</v>
+      </c>
+      <c r="R2">
+        <v>1.07955207220888E-2</v>
+      </c>
+      <c r="S2">
+        <v>1.2224842829034801E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>0.2128</v>
+        <v>0.21279999999999999</v>
       </c>
       <c r="C3">
-        <v>0.0916857142857142</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.0340240350044375</v>
+        <v>9.1685714285714204E-2</v>
       </c>
       <c r="E3">
-        <v>0.0293686442129214</v>
+        <v>3.40240350044375E-2</v>
       </c>
       <c r="F3">
-        <v>0.2160428571428571</v>
+        <v>0</v>
       </c>
       <c r="G3">
+        <v>2.9368644212921399E-2</v>
+      </c>
+      <c r="H3">
+        <v>0.21604285714285709</v>
+      </c>
+      <c r="I3">
         <v>0.2126166666666667</v>
       </c>
-      <c r="H3">
-        <v>0.2126166666666667</v>
-      </c>
-      <c r="I3">
-        <v>0.0335000796735657</v>
-      </c>
       <c r="J3">
-        <v>0.0304324106632048</v>
+        <v>0.17378571428571429</v>
       </c>
       <c r="K3">
-        <v>0.0304324106632048</v>
+        <v>3.3500079673565698E-2</v>
       </c>
       <c r="L3">
-        <v>0.1990873015873016</v>
+        <v>3.04324106632048E-2</v>
       </c>
       <c r="M3">
+        <v>3.1453914215686898E-2</v>
+      </c>
+      <c r="N3">
+        <v>0.19908730158730159</v>
+      </c>
+      <c r="O3">
         <v>0.1840396825396825</v>
       </c>
-      <c r="N3">
-        <v>0.1840396825396825</v>
-      </c>
-      <c r="O3">
-        <v>0.0346461618407768</v>
-      </c>
       <c r="P3">
-        <v>0.0267363020725282</v>
+        <v>0.20418253968253969</v>
       </c>
       <c r="Q3">
-        <v>0.0267363020725282</v>
+        <v>3.4646161840776797E-2</v>
+      </c>
+      <c r="R3">
+        <v>2.6736302072528199E-2</v>
+      </c>
+      <c r="S3">
+        <v>3.4322711129908201E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>0.334875</v>
+        <v>0.33487499999999998</v>
       </c>
       <c r="C4">
-        <v>0.265375</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.0428291612522522</v>
+        <v>0.26537500000000003</v>
       </c>
       <c r="E4">
-        <v>0.06690503330948171</v>
+        <v>4.2829161252252203E-2</v>
       </c>
       <c r="F4">
-        <v>0.1733125</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0.1665</v>
+        <v>6.6905033309481707E-2</v>
       </c>
       <c r="H4">
-        <v>0.1665</v>
+        <v>0.17331250000000001</v>
       </c>
       <c r="I4">
-        <v>0.08193279910358491</v>
+        <v>0.16650000000000001</v>
       </c>
       <c r="J4">
-        <v>0.0220510140860283</v>
+        <v>0.18331249999999999</v>
       </c>
       <c r="K4">
-        <v>0.0220510140860283</v>
+        <v>8.1932799103584905E-2</v>
       </c>
       <c r="L4">
-        <v>0.2342708333333333</v>
+        <v>2.20510140860283E-2</v>
       </c>
       <c r="M4">
-        <v>0.2337708333333333</v>
+        <v>9.6984757012418807E-2</v>
       </c>
       <c r="N4">
-        <v>0.2337708333333333</v>
+        <v>0.23427083333333329</v>
       </c>
       <c r="O4">
-        <v>0.0589741427076464</v>
+        <v>0.23377083333333329</v>
       </c>
       <c r="P4">
-        <v>0.0759957842931045</v>
+        <v>0.22502083333333331</v>
       </c>
       <c r="Q4">
-        <v>0.0759957842931045</v>
+        <v>5.89741427076464E-2</v>
+      </c>
+      <c r="R4">
+        <v>7.5995784293104496E-2</v>
+      </c>
+      <c r="S4">
+        <v>0.10653821136251571</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>0.2253240223463687</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>0.1154189944134078</v>
       </c>
-      <c r="D5">
-        <v>0.0132233095837899</v>
-      </c>
       <c r="E5">
-        <v>0.0126303505116116</v>
+        <v>1.3223309583789899E-2</v>
       </c>
       <c r="F5">
-        <v>0.2076792929292929</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.1850323529411764</v>
+        <v>1.2630350511611601E-2</v>
       </c>
       <c r="H5">
-        <v>0.1850323529411764</v>
+        <v>0.20780555555555549</v>
       </c>
       <c r="I5">
-        <v>0.0134238781000222</v>
+        <v>0.18517941176470579</v>
       </c>
       <c r="J5">
-        <v>0.012055250004402</v>
+        <v>0.16030555555555551</v>
       </c>
       <c r="K5">
-        <v>0.012055250004402</v>
+        <v>1.34170572563961E-2</v>
       </c>
       <c r="L5">
+        <v>1.2048995224502999E-2</v>
+      </c>
+      <c r="M5">
+        <v>1.2386591773217799E-2</v>
+      </c>
+      <c r="N5">
         <v>0.1937799145299145</v>
       </c>
-      <c r="M5">
-        <v>0.1694363247863248</v>
-      </c>
-      <c r="N5">
-        <v>0.1694363247863248</v>
-      </c>
       <c r="O5">
-        <v>0.0110285750778723</v>
+        <v>0.16943632478632481</v>
       </c>
       <c r="P5">
-        <v>0.0099439697445949</v>
+        <v>0.18848760683760679</v>
       </c>
       <c r="Q5">
-        <v>0.0099439697445949</v>
+        <v>1.1028575077872299E-2</v>
+      </c>
+      <c r="R5">
+        <v>9.9439697445949E-3</v>
+      </c>
+      <c r="S5">
+        <v>1.14232188759778E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>